<commit_message>
wip diamand of Leavitt
</commit_message>
<xml_diff>
--- a/Phase-1-preparation/McKinsey-Steps/McKinsey-Steps.xlsx
+++ b/Phase-1-preparation/McKinsey-Steps/McKinsey-Steps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelkonrath/Documents/Epitech/ProjetMSC1/Gotham/gotham_2020_20/Phase-1-preparation/McKinsey-Steps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{8C027A47-CB69-484E-BFCA-C1F6623AD192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{51177F61-D695-3649-BFB5-7FAE4D66B520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17920" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Situation" sheetId="1" r:id="rId1"/>
@@ -29,11 +29,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>[Élément]</t>
   </si>
   <si>
+    <t>[Note]</t>
+  </si>
+  <si>
     <t>McKinsey 7S : Current Situation</t>
   </si>
   <si>
@@ -64,10 +67,19 @@
     <t>Shared vales :</t>
   </si>
   <si>
+    <t xml:space="preserve">Etat actuel des chose </t>
+  </si>
+  <si>
     <t>YES</t>
   </si>
   <si>
     <t>Aligned ? YES/NO</t>
+  </si>
+  <si>
+    <t>McKinsey 7S : Readiness for Future</t>
+  </si>
+  <si>
+    <t>Desired Situation</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -191,7 +203,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -211,6 +223,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -228,6 +243,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -260,14 +278,14 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -305,7 +323,8 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="Tâches" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="2" defaultTableStyle="Tâches" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Style de tableau 1" pivot="0" count="0" xr9:uid="{0EC40D14-102D-BE43-96E7-13214A8729FD}"/>
     <tableStyle name="Tâches" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="8"/>
       <tableStyleElement type="headerRow" dxfId="7"/>
@@ -328,8 +347,8 @@
   <autoFilter ref="B6:D11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="7S" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Comment" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Aligned ? YES/NO" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Comment" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Aligned ? YES/NO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Tâches" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -341,12 +360,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{780606AE-D964-C54C-B565-2F0F4AFFF31B}" name="Tâches4" displayName="Tâches4" ref="B6:D11" totalsRowShown="0">
-  <autoFilter ref="B6:D11" xr:uid="{BC1296E1-C6B0-E24A-9CE2-C7559377F420}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7EE65E47-007A-F841-9ECB-F76C09584F11}" name="Tâches2" displayName="Tâches2" ref="B6:D10" totalsRowShown="0">
+  <autoFilter ref="B6:D10" xr:uid="{6EA1C08A-F6DC-114D-AA3D-6A6EDEA9EAAC}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8D25600C-BAB3-9C4C-94BE-A4030A800343}" name="7S" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{92DE3074-D58C-A049-A8E4-67E0A08567CF}" name="Comment" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{96F34E42-147A-DE42-AACD-0668414B190B}" name="Aligned ? YES/NO" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D7BAA330-F44B-D44F-91EE-DA1B10506B18}" name="7S" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EC34F5A8-6792-E94C-8E00-93E6CECB95B5}" name="Comment" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{79978328-3BCF-A043-BA7F-DB281D401844}" name="Aligned ? YES/NO" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Tâches" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -626,28 +645,28 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="A8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="18" style="11" customWidth="1"/>
+    <col min="2" max="2" width="18" style="12" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="6"/>
     </row>
@@ -668,88 +687,88 @@
     </row>
     <row r="6" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="8" spans="1:5" ht="125" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="10" t="s">
-        <v>6</v>
+      <c r="B8" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>16</v>
+      <c r="D8" s="20" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="146" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="10" t="s">
-        <v>7</v>
+      <c r="B9" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>16</v>
+      <c r="D9" s="20" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="160" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>16</v>
+      <c r="B10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="10" t="s">
-        <v>8</v>
+      <c r="B11" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="18" t="s">
-        <v>16</v>
+      <c r="D11" s="20" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>16</v>
+      <c r="B12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="176" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="19" t="s">
+      <c r="B13" s="14" t="s">
         <v>11</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -767,30 +786,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1AD43A6-260B-464F-A132-9EF503715C96}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="18" style="11" customWidth="1"/>
+    <col min="2" max="2" width="18" style="12" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D2" s="6"/>
     </row>
@@ -811,92 +830,84 @@
     </row>
     <row r="6" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="125" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="10" t="s">
-        <v>6</v>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="146" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="10" t="s">
-        <v>7</v>
+      <c r="D8" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="160" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
+      <c r="D9" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="176" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
+      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="19" t="s">
+      <c r="C11" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
         <v>11</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>